<commit_message>
Include tech_fuel combination and use for mapping
</commit_message>
<xml_diff>
--- a/raw_data_input/assumptions/Pietzcker_et_al_2021_technology_assumptions.xlsx
+++ b/raw_data_input/assumptions/Pietzcker_et_al_2021_technology_assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20388"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\POMMES_public\pommes-data\raw_data_input\assumptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8667D5F3-2AA5-4516-8D0D-04C3BC64168A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2F4555-1566-4DB7-9EAA-D2B498E8886C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" activeTab="1" xr2:uid="{6742E402-8328-41E3-BF2E-C104FAD388A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6345" xr2:uid="{6742E402-8328-41E3-BF2E-C104FAD388A3}"/>
   </bookViews>
   <sheets>
     <sheet name="investment_expenses" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Lignite</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Lignite CCS</t>
-  </si>
-  <si>
-    <t>Gas CCS</t>
   </si>
   <si>
     <t>Wind Onshore</t>
@@ -540,24 +537,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9CB2BA-1E70-484D-BDB9-121441E8BBD0}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -568,19 +565,19 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -589,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -621,7 +618,7 @@
         <v>6250</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -653,7 +650,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -685,7 +682,7 @@
         <v>4750</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2025</v>
       </c>
@@ -717,7 +714,7 @@
         <v>4750</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2030</v>
       </c>
@@ -749,7 +746,7 @@
         <v>4750</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2035</v>
       </c>
@@ -781,7 +778,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2040</v>
       </c>
@@ -813,7 +810,7 @@
         <v>4450</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2045</v>
       </c>
@@ -845,7 +842,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2050</v>
       </c>
@@ -886,69 +883,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EFB6C1-F317-4ACD-B1ED-BB22E643BD70}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>39</v>
       </c>
       <c r="B3">
         <v>7000</v>
@@ -972,7 +969,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -980,7 +977,7 @@
         <v>1800</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -998,7 +995,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1021,7 +1018,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1026,7 @@
         <v>2100</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -1047,7 +1044,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1070,15 +1067,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>900</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1096,9 +1093,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>52</v>
@@ -1119,9 +1116,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>400</v>
@@ -1145,9 +1142,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11">
         <v>400</v>
@@ -1171,9 +1168,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>945</v>
@@ -1197,9 +1194,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>420</v>
@@ -1223,9 +1220,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>45</v>
@@ -1246,9 +1243,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>2000</v>
@@ -1272,9 +1269,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16">
         <v>900</v>
@@ -1298,9 +1295,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17">
         <v>2000</v>
@@ -1324,7 +1321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1347,9 +1344,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19">
         <v>2500</v>
@@ -1373,9 +1370,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>100</v>
@@ -1396,9 +1393,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>100</v>
@@ -1419,7 +1416,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1442,7 +1439,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1478,40 +1475,40 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>18</v>
       </c>
       <c r="B2">
         <v>1129</v>
@@ -1532,9 +1529,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1549,9 +1546,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -1582,20 +1579,20 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
       </c>
       <c r="C1">
         <v>2010</v>
@@ -1622,15 +1619,15 @@
         <v>2045</v>
       </c>
       <c r="K1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
       <c r="C2">
         <v>678</v>
@@ -1660,9 +1657,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>802</v>
@@ -1692,12 +1689,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>1595</v>

</xml_diff>